<commit_message>
Added counts at the bottom of outputs/declined
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="135">
   <si>
     <t xml:space="preserve">Name: </t>
   </si>
@@ -178,6 +178,9 @@
     <t>Renu Srivathsa</t>
   </si>
   <si>
+    <t>Count: 46</t>
+  </si>
+  <si>
     <t>IAIM</t>
   </si>
   <si>
@@ -335,6 +338,9 @@
   </si>
   <si>
     <t>Prabhav Nadella</t>
+  </si>
+  <si>
+    <t>Count: 38</t>
   </si>
   <si>
     <t>Malladi Sreeram Prasad</t>
@@ -776,7 +782,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -810,10 +816,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -822,7 +828,7 @@
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -833,10 +839,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E3">
         <v>15</v>
@@ -845,7 +851,7 @@
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -856,10 +862,10 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -868,7 +874,7 @@
         <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -879,10 +885,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -891,7 +897,7 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -902,10 +908,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -914,7 +920,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -925,10 +931,10 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E7">
         <v>15</v>
@@ -937,7 +943,7 @@
         <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -948,10 +954,10 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E8">
         <v>15</v>
@@ -960,7 +966,7 @@
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -971,10 +977,10 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -983,7 +989,7 @@
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -994,10 +1000,10 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E10">
         <v>5</v>
@@ -1006,7 +1012,7 @@
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1017,10 +1023,10 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E11">
         <v>15</v>
@@ -1029,7 +1035,7 @@
         <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1040,10 +1046,10 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E12">
         <v>15</v>
@@ -1052,7 +1058,7 @@
         <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1063,10 +1069,10 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E13">
         <v>10</v>
@@ -1075,7 +1081,7 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1086,10 +1092,10 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E14">
         <v>10</v>
@@ -1098,7 +1104,7 @@
         <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1109,10 +1115,10 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E15">
         <v>20</v>
@@ -1121,7 +1127,7 @@
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1132,10 +1138,10 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E16">
         <v>10</v>
@@ -1144,7 +1150,7 @@
         <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1155,10 +1161,10 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E17">
         <v>30</v>
@@ -1167,7 +1173,7 @@
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1178,10 +1184,10 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E18">
         <v>5</v>
@@ -1190,7 +1196,7 @@
         <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1201,10 +1207,10 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E19">
         <v>25</v>
@@ -1213,7 +1219,7 @@
         <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1224,10 +1230,10 @@
         <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E20">
         <v>30</v>
@@ -1236,7 +1242,7 @@
         <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1247,10 +1253,10 @@
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E21">
         <v>15</v>
@@ -1259,7 +1265,7 @@
         <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1270,10 +1276,10 @@
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E22">
         <v>15</v>
@@ -1282,7 +1288,7 @@
         <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1293,10 +1299,10 @@
         <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E23">
         <v>10</v>
@@ -1305,7 +1311,7 @@
         <v>11</v>
       </c>
       <c r="G23" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1316,10 +1322,10 @@
         <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E24">
         <v>30</v>
@@ -1328,7 +1334,7 @@
         <v>11</v>
       </c>
       <c r="G24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1339,10 +1345,10 @@
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E25">
         <v>10</v>
@@ -1351,7 +1357,7 @@
         <v>11</v>
       </c>
       <c r="G25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1362,10 +1368,10 @@
         <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E26">
         <v>20</v>
@@ -1374,7 +1380,7 @@
         <v>11</v>
       </c>
       <c r="G26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1385,10 +1391,10 @@
         <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E27">
         <v>10</v>
@@ -1397,7 +1403,7 @@
         <v>11</v>
       </c>
       <c r="G27" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1408,10 +1414,10 @@
         <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E28">
         <v>10</v>
@@ -1420,7 +1426,7 @@
         <v>11</v>
       </c>
       <c r="G28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1431,10 +1437,10 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E29">
         <v>10</v>
@@ -1443,7 +1449,7 @@
         <v>11</v>
       </c>
       <c r="G29" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1454,10 +1460,10 @@
         <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E30">
         <v>10</v>
@@ -1466,7 +1472,7 @@
         <v>11</v>
       </c>
       <c r="G30" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1477,10 +1483,10 @@
         <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D31" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E31">
         <v>30</v>
@@ -1489,7 +1495,7 @@
         <v>11</v>
       </c>
       <c r="G31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1500,10 +1506,10 @@
         <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E32">
         <v>20</v>
@@ -1512,7 +1518,7 @@
         <v>11</v>
       </c>
       <c r="G32" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1523,10 +1529,10 @@
         <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E33">
         <v>15</v>
@@ -1535,7 +1541,7 @@
         <v>11</v>
       </c>
       <c r="G33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1546,10 +1552,10 @@
         <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D34" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E34">
         <v>20</v>
@@ -1558,7 +1564,7 @@
         <v>11</v>
       </c>
       <c r="G34" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1569,10 +1575,10 @@
         <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E35">
         <v>25</v>
@@ -1581,7 +1587,7 @@
         <v>11</v>
       </c>
       <c r="G35" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1592,10 +1598,10 @@
         <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D36" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E36">
         <v>10</v>
@@ -1604,7 +1610,7 @@
         <v>11</v>
       </c>
       <c r="G36" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1615,10 +1621,10 @@
         <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D37" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E37">
         <v>20</v>
@@ -1627,7 +1633,7 @@
         <v>11</v>
       </c>
       <c r="G37" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1638,10 +1644,10 @@
         <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D38" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E38">
         <v>25</v>
@@ -1650,7 +1656,7 @@
         <v>11</v>
       </c>
       <c r="G38" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1661,10 +1667,10 @@
         <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D39" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E39">
         <v>15</v>
@@ -1673,7 +1679,7 @@
         <v>11</v>
       </c>
       <c r="G39" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1684,10 +1690,10 @@
         <v>44</v>
       </c>
       <c r="C40" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D40" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E40">
         <v>20</v>
@@ -1696,7 +1702,7 @@
         <v>10</v>
       </c>
       <c r="G40" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1707,10 +1713,10 @@
         <v>45</v>
       </c>
       <c r="C41" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D41" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E41">
         <v>15</v>
@@ -1719,7 +1725,7 @@
         <v>10</v>
       </c>
       <c r="G41" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1730,10 +1736,10 @@
         <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D42" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E42">
         <v>10</v>
@@ -1742,7 +1748,7 @@
         <v>9</v>
       </c>
       <c r="G42" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1753,10 +1759,10 @@
         <v>47</v>
       </c>
       <c r="C43" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D43" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E43">
         <v>15</v>
@@ -1765,7 +1771,7 @@
         <v>8</v>
       </c>
       <c r="G43" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1776,10 +1782,10 @@
         <v>48</v>
       </c>
       <c r="C44" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D44" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E44">
         <v>20</v>
@@ -1788,7 +1794,7 @@
         <v>7</v>
       </c>
       <c r="G44" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1799,10 +1805,10 @@
         <v>49</v>
       </c>
       <c r="C45" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D45" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E45">
         <v>5</v>
@@ -1811,7 +1817,7 @@
         <v>7</v>
       </c>
       <c r="G45" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1822,10 +1828,10 @@
         <v>50</v>
       </c>
       <c r="C46" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D46" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E46">
         <v>10</v>
@@ -1834,7 +1840,7 @@
         <v>6</v>
       </c>
       <c r="G46" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1845,10 +1851,10 @@
         <v>51</v>
       </c>
       <c r="C47" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D47" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E47">
         <v>15</v>
@@ -1857,7 +1863,20 @@
         <v>6</v>
       </c>
       <c r="G47" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1867,7 +1886,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1881,10 +1900,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -1893,7 +1912,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -1901,25 +1920,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G2">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1927,25 +1946,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G3">
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1953,25 +1972,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G4">
         <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1979,25 +1998,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E5">
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G5">
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2005,25 +2024,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G6">
         <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2031,25 +2050,25 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G7">
         <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2057,25 +2076,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E8">
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G8">
         <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2083,25 +2102,25 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G9">
         <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2109,25 +2128,25 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G10">
         <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2135,25 +2154,25 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E11">
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G11">
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2161,25 +2180,25 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E12">
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G12">
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2187,25 +2206,25 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E13">
         <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G13">
         <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2213,25 +2232,25 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E14">
         <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G14">
         <v>10</v>
       </c>
       <c r="H14" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2239,25 +2258,25 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E15">
         <v>30</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G15">
         <v>10</v>
       </c>
       <c r="H15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2265,25 +2284,25 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E16">
         <v>30</v>
       </c>
       <c r="F16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G16">
         <v>10</v>
       </c>
       <c r="H16" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2291,25 +2310,25 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E17">
         <v>30</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G17">
         <v>10</v>
       </c>
       <c r="H17" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2317,25 +2336,25 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C18" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E18">
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G18">
         <v>10</v>
       </c>
       <c r="H18" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2343,25 +2362,25 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C19" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E19">
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G19">
         <v>10</v>
       </c>
       <c r="H19" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2369,25 +2388,25 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E20">
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G20">
         <v>10</v>
       </c>
       <c r="H20" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2395,25 +2414,25 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E21">
         <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G21">
         <v>10</v>
       </c>
       <c r="H21" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2421,25 +2440,25 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E22">
         <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G22">
         <v>9</v>
       </c>
       <c r="H22" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2447,25 +2466,25 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E23">
         <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G23">
         <v>9</v>
       </c>
       <c r="H23" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2473,25 +2492,25 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E24">
         <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G24">
         <v>9</v>
       </c>
       <c r="H24" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2499,25 +2518,25 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E25">
         <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G25">
         <v>9</v>
       </c>
       <c r="H25" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2525,25 +2544,25 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C26" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E26">
         <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G26">
         <v>9</v>
       </c>
       <c r="H26" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2551,25 +2570,25 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E27">
         <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G27">
         <v>9</v>
       </c>
       <c r="H27" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2577,25 +2596,25 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E28">
         <v>20</v>
       </c>
       <c r="F28" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G28">
         <v>9</v>
       </c>
       <c r="H28" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2603,25 +2622,25 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E29">
         <v>20</v>
       </c>
       <c r="F29" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G29">
         <v>9</v>
       </c>
       <c r="H29" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2629,25 +2648,25 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C30" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D30" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E30">
         <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G30">
         <v>8</v>
       </c>
       <c r="H30" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2655,25 +2674,25 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C31" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E31">
         <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G31">
         <v>8</v>
       </c>
       <c r="H31" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2681,25 +2700,25 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D32" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E32">
         <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G32">
         <v>8</v>
       </c>
       <c r="H32" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2707,25 +2726,25 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D33" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E33">
         <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G33">
         <v>8</v>
       </c>
       <c r="H33" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2733,25 +2752,25 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C34" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D34" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E34">
         <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G34">
         <v>8</v>
       </c>
       <c r="H34" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2759,25 +2778,25 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E35">
         <v>10</v>
       </c>
       <c r="F35" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G35">
         <v>8</v>
       </c>
       <c r="H35" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2785,25 +2804,25 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C36" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D36" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E36">
         <v>30</v>
       </c>
       <c r="F36" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G36">
         <v>6</v>
       </c>
       <c r="H36" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2811,25 +2830,25 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E37">
         <v>30</v>
       </c>
       <c r="F37" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G37">
         <v>6</v>
       </c>
       <c r="H37" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2837,25 +2856,25 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C38" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D38" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E38">
         <v>10</v>
       </c>
       <c r="F38" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G38">
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2863,25 +2882,38 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C39" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E39">
         <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G39">
         <v>5</v>
       </c>
       <c r="H39" t="s">
-        <v>120</v>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2922,7 +2954,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D2">
         <v>15</v>
@@ -2931,7 +2963,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2942,7 +2974,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -2951,7 +2983,7 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2962,7 +2994,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D4">
         <v>15</v>
@@ -2971,7 +3003,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2982,7 +3014,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -2991,7 +3023,7 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3002,7 +3034,7 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D6">
         <v>15</v>
@@ -3011,7 +3043,7 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3022,7 +3054,7 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -3031,7 +3063,7 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3042,7 +3074,7 @@
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -3051,7 +3083,7 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3062,7 +3094,7 @@
         <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D9">
         <v>25</v>
@@ -3071,7 +3103,7 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3082,7 +3114,7 @@
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D10">
         <v>20</v>
@@ -3091,7 +3123,7 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3102,7 +3134,7 @@
         <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D11">
         <v>25</v>
@@ -3111,7 +3143,7 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3152,7 +3184,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D2">
         <v>20</v>
@@ -3161,7 +3193,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3172,7 +3204,7 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -3181,7 +3213,7 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3192,7 +3224,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -3201,7 +3233,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3212,7 +3244,7 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D5">
         <v>30</v>
@@ -3221,7 +3253,7 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3232,7 +3264,7 @@
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D6">
         <v>15</v>
@@ -3241,7 +3273,7 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3252,7 +3284,7 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -3261,7 +3293,7 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3272,7 +3304,7 @@
         <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D8">
         <v>15</v>
@@ -3281,7 +3313,7 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3292,7 +3324,7 @@
         <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -3301,7 +3333,7 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3342,7 +3374,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -3351,7 +3383,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3362,7 +3394,7 @@
         <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -3371,7 +3403,7 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3382,7 +3414,7 @@
         <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D4">
         <v>15</v>
@@ -3391,7 +3423,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3402,7 +3434,7 @@
         <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D5">
         <v>30</v>
@@ -3411,7 +3443,7 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3422,7 +3454,7 @@
         <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -3431,7 +3463,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3442,7 +3474,7 @@
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D7">
         <v>20</v>
@@ -3451,7 +3483,7 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3462,7 +3494,7 @@
         <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D8">
         <v>20</v>
@@ -3471,7 +3503,7 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3482,7 +3514,7 @@
         <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -3491,7 +3523,7 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3502,7 +3534,7 @@
         <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D10">
         <v>20</v>
@@ -3511,7 +3543,7 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3522,7 +3554,7 @@
         <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D11">
         <v>15</v>
@@ -3531,7 +3563,7 @@
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3572,7 +3604,7 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D2">
         <v>15</v>
@@ -3581,7 +3613,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3592,7 +3624,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -3601,7 +3633,7 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3612,7 +3644,7 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D4">
         <v>20</v>
@@ -3621,7 +3653,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3632,7 +3664,7 @@
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D5">
         <v>25</v>
@@ -3641,7 +3673,7 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3652,7 +3684,7 @@
         <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D6">
         <v>30</v>
@@ -3661,7 +3693,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3672,7 +3704,7 @@
         <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D7">
         <v>15</v>
@@ -3681,7 +3713,7 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3692,7 +3724,7 @@
         <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -3701,7 +3733,7 @@
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3712,7 +3744,7 @@
         <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -3721,7 +3753,7 @@
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3732,7 +3764,7 @@
         <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D10">
         <v>15</v>
@@ -3741,7 +3773,7 @@
         <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3782,7 +3814,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D2">
         <v>15</v>
@@ -3791,7 +3823,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3802,7 +3834,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D3">
         <v>15</v>
@@ -3811,7 +3843,7 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3822,7 +3854,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -3831,7 +3863,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3842,7 +3874,7 @@
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D5">
         <v>30</v>
@@ -3851,7 +3883,7 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3862,7 +3894,7 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -3871,7 +3903,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3882,7 +3914,7 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D7">
         <v>20</v>
@@ -3891,7 +3923,7 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3902,7 +3934,7 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -3911,7 +3943,7 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3922,7 +3954,7 @@
         <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D9">
         <v>15</v>
@@ -3931,7 +3963,7 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3942,7 +3974,7 @@
         <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D10">
         <v>20</v>
@@ -3951,7 +3983,7 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some more changes
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sashw\Documents\CCC Performance Assignment Program\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Outputs" sheetId="1" r:id="rId1"/>
@@ -15,7 +20,7 @@
     <sheet name="May 2021" sheetId="6" r:id="rId6"/>
     <sheet name="June 2021" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -178,9 +183,6 @@
     <t>Renu Srivathsa</t>
   </si>
   <si>
-    <t>Count: 46</t>
-  </si>
-  <si>
     <t>IAIM</t>
   </si>
   <si>
@@ -340,9 +342,6 @@
     <t>Prabhav Nadella</t>
   </si>
   <si>
-    <t>Count: 38</t>
-  </si>
-  <si>
     <t>Malladi Sreeram Prasad</t>
   </si>
   <si>
@@ -425,13 +424,19 @@
   </si>
   <si>
     <t>For May, the school limit for IAIM is reached</t>
+  </si>
+  <si>
+    <t>COUNT = 19</t>
+  </si>
+  <si>
+    <t>COUNT = 46</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,6 +499,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -540,7 +553,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -572,9 +585,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -606,6 +620,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -781,14 +796,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -808,7 +825,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -816,10 +833,10 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -828,10 +845,10 @@
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -839,10 +856,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3">
         <v>15</v>
@@ -851,10 +868,10 @@
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -862,10 +879,10 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -874,10 +891,10 @@
         <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -885,10 +902,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -897,10 +914,10 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -908,10 +925,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -920,10 +937,10 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -931,10 +948,10 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E7">
         <v>15</v>
@@ -943,10 +960,10 @@
         <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -954,10 +971,10 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8">
         <v>15</v>
@@ -966,10 +983,10 @@
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -977,10 +994,10 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E9">
         <v>10</v>
@@ -989,10 +1006,10 @@
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1000,10 +1017,10 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E10">
         <v>5</v>
@@ -1012,10 +1029,10 @@
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1023,10 +1040,10 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E11">
         <v>15</v>
@@ -1035,10 +1052,10 @@
         <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1046,10 +1063,10 @@
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E12">
         <v>15</v>
@@ -1058,10 +1075,10 @@
         <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1069,10 +1086,10 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13">
         <v>10</v>
@@ -1081,10 +1098,10 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1092,10 +1109,10 @@
         <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E14">
         <v>10</v>
@@ -1104,10 +1121,10 @@
         <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1115,10 +1132,10 @@
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E15">
         <v>20</v>
@@ -1127,10 +1144,10 @@
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1138,10 +1155,10 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E16">
         <v>10</v>
@@ -1150,10 +1167,10 @@
         <v>12</v>
       </c>
       <c r="G16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1161,10 +1178,10 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E17">
         <v>30</v>
@@ -1173,10 +1190,10 @@
         <v>12</v>
       </c>
       <c r="G17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1184,10 +1201,10 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E18">
         <v>5</v>
@@ -1196,10 +1213,10 @@
         <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1207,10 +1224,10 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E19">
         <v>25</v>
@@ -1219,10 +1236,10 @@
         <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1230,10 +1247,10 @@
         <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E20">
         <v>30</v>
@@ -1242,10 +1259,10 @@
         <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1253,10 +1270,10 @@
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E21">
         <v>15</v>
@@ -1265,10 +1282,10 @@
         <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1276,10 +1293,10 @@
         <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E22">
         <v>15</v>
@@ -1288,10 +1305,10 @@
         <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1299,10 +1316,10 @@
         <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E23">
         <v>10</v>
@@ -1311,10 +1328,10 @@
         <v>11</v>
       </c>
       <c r="G23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1322,10 +1339,10 @@
         <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E24">
         <v>30</v>
@@ -1334,10 +1351,10 @@
         <v>11</v>
       </c>
       <c r="G24" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1345,10 +1362,10 @@
         <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E25">
         <v>10</v>
@@ -1357,10 +1374,10 @@
         <v>11</v>
       </c>
       <c r="G25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1368,10 +1385,10 @@
         <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E26">
         <v>20</v>
@@ -1380,10 +1397,10 @@
         <v>11</v>
       </c>
       <c r="G26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1391,10 +1408,10 @@
         <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E27">
         <v>10</v>
@@ -1403,10 +1420,10 @@
         <v>11</v>
       </c>
       <c r="G27" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1414,10 +1431,10 @@
         <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E28">
         <v>10</v>
@@ -1426,10 +1443,10 @@
         <v>11</v>
       </c>
       <c r="G28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1437,10 +1454,10 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E29">
         <v>10</v>
@@ -1449,10 +1466,10 @@
         <v>11</v>
       </c>
       <c r="G29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1460,10 +1477,10 @@
         <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E30">
         <v>10</v>
@@ -1472,10 +1489,10 @@
         <v>11</v>
       </c>
       <c r="G30" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1483,10 +1500,10 @@
         <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E31">
         <v>30</v>
@@ -1495,10 +1512,10 @@
         <v>11</v>
       </c>
       <c r="G31" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1506,10 +1523,10 @@
         <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E32">
         <v>20</v>
@@ -1518,10 +1535,10 @@
         <v>11</v>
       </c>
       <c r="G32" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1529,10 +1546,10 @@
         <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E33">
         <v>15</v>
@@ -1541,10 +1558,10 @@
         <v>11</v>
       </c>
       <c r="G33" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1552,10 +1569,10 @@
         <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E34">
         <v>20</v>
@@ -1564,10 +1581,10 @@
         <v>11</v>
       </c>
       <c r="G34" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1575,10 +1592,10 @@
         <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E35">
         <v>25</v>
@@ -1587,10 +1604,10 @@
         <v>11</v>
       </c>
       <c r="G35" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1598,10 +1615,10 @@
         <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E36">
         <v>10</v>
@@ -1610,10 +1627,10 @@
         <v>11</v>
       </c>
       <c r="G36" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1621,10 +1638,10 @@
         <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E37">
         <v>20</v>
@@ -1633,10 +1650,10 @@
         <v>11</v>
       </c>
       <c r="G37" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1644,10 +1661,10 @@
         <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E38">
         <v>25</v>
@@ -1656,10 +1673,10 @@
         <v>11</v>
       </c>
       <c r="G38" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1667,10 +1684,10 @@
         <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E39">
         <v>15</v>
@@ -1679,10 +1696,10 @@
         <v>11</v>
       </c>
       <c r="G39" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1690,10 +1707,10 @@
         <v>44</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E40">
         <v>20</v>
@@ -1702,10 +1719,10 @@
         <v>10</v>
       </c>
       <c r="G40" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1713,10 +1730,10 @@
         <v>45</v>
       </c>
       <c r="C41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E41">
         <v>15</v>
@@ -1725,10 +1742,10 @@
         <v>10</v>
       </c>
       <c r="G41" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1736,10 +1753,10 @@
         <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E42">
         <v>10</v>
@@ -1748,10 +1765,10 @@
         <v>9</v>
       </c>
       <c r="G42" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1759,10 +1776,10 @@
         <v>47</v>
       </c>
       <c r="C43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E43">
         <v>15</v>
@@ -1771,10 +1788,10 @@
         <v>8</v>
       </c>
       <c r="G43" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1782,10 +1799,10 @@
         <v>48</v>
       </c>
       <c r="C44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E44">
         <v>20</v>
@@ -1794,10 +1811,10 @@
         <v>7</v>
       </c>
       <c r="G44" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1805,10 +1822,10 @@
         <v>49</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E45">
         <v>5</v>
@@ -1817,10 +1834,10 @@
         <v>7</v>
       </c>
       <c r="G45" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1828,10 +1845,10 @@
         <v>50</v>
       </c>
       <c r="C46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E46">
         <v>10</v>
@@ -1840,10 +1857,10 @@
         <v>6</v>
       </c>
       <c r="G46" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1851,10 +1868,10 @@
         <v>51</v>
       </c>
       <c r="C47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E47">
         <v>15</v>
@@ -1863,20 +1880,20 @@
         <v>6</v>
       </c>
       <c r="G47" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1885,14 +1902,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1900,10 +1919,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -1912,1008 +1931,1008 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G2">
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G3">
         <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G4">
         <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E5">
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G5">
         <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G6">
         <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G7">
         <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E8">
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G8">
         <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G9">
         <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E10">
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G10">
         <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E11">
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G11">
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E12">
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G12">
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E13">
         <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G13">
         <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E14">
         <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G14">
         <v>10</v>
       </c>
       <c r="H14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E15">
         <v>30</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G15">
         <v>10</v>
       </c>
       <c r="H15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16">
         <v>30</v>
       </c>
       <c r="F16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G16">
         <v>10</v>
       </c>
       <c r="H16" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E17">
         <v>30</v>
       </c>
       <c r="F17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G17">
         <v>10</v>
       </c>
       <c r="H17" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E18">
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G18">
         <v>10</v>
       </c>
       <c r="H18" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E19">
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G19">
         <v>10</v>
       </c>
       <c r="H19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E20">
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G20">
         <v>10</v>
       </c>
       <c r="H20" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E21">
         <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G21">
         <v>10</v>
       </c>
       <c r="H21" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E22">
         <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G22">
         <v>9</v>
       </c>
       <c r="H22" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E23">
         <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G23">
         <v>9</v>
       </c>
       <c r="H23" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E24">
         <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G24">
         <v>9</v>
       </c>
       <c r="H24" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E25">
         <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G25">
         <v>9</v>
       </c>
       <c r="H25" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C26" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E26">
         <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G26">
         <v>9</v>
       </c>
       <c r="H26" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C27" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E27">
         <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G27">
         <v>9</v>
       </c>
       <c r="H27" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E28">
         <v>20</v>
       </c>
       <c r="F28" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G28">
         <v>9</v>
       </c>
       <c r="H28" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E29">
         <v>20</v>
       </c>
       <c r="F29" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G29">
         <v>9</v>
       </c>
       <c r="H29" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C30" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E30">
         <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G30">
         <v>8</v>
       </c>
       <c r="H30" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E31">
         <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G31">
         <v>8</v>
       </c>
       <c r="H31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E32">
         <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G32">
         <v>8</v>
       </c>
       <c r="H32" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E33">
         <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G33">
         <v>8</v>
       </c>
       <c r="H33" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" t="s">
         <v>114</v>
       </c>
-      <c r="D34" t="s">
-        <v>116</v>
-      </c>
       <c r="E34">
         <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G34">
         <v>8</v>
       </c>
       <c r="H34" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E35">
         <v>10</v>
       </c>
       <c r="F35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G35">
         <v>8</v>
       </c>
       <c r="H35" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E36">
         <v>30</v>
       </c>
       <c r="F36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G36">
         <v>6</v>
       </c>
       <c r="H36" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E37">
         <v>30</v>
       </c>
       <c r="F37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G37">
         <v>6</v>
       </c>
       <c r="H37" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E38">
         <v>10</v>
       </c>
       <c r="F38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G38">
         <v>5</v>
       </c>
       <c r="H38" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C39" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E39">
         <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G39">
         <v>5</v>
       </c>
       <c r="H39" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2922,14 +2941,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2946,7 +2965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2954,7 +2973,7 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2">
         <v>15</v>
@@ -2963,10 +2982,10 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2974,7 +2993,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -2983,10 +3002,10 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2994,7 +3013,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4">
         <v>15</v>
@@ -3003,10 +3022,10 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3014,7 +3033,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -3023,10 +3042,10 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3034,7 +3053,7 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6">
         <v>15</v>
@@ -3043,10 +3062,10 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3054,7 +3073,7 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -3063,10 +3082,10 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3074,7 +3093,7 @@
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -3083,10 +3102,10 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3094,7 +3113,7 @@
         <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9">
         <v>25</v>
@@ -3103,10 +3122,10 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3114,7 +3133,7 @@
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10">
         <v>20</v>
@@ -3123,10 +3142,10 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3134,7 +3153,7 @@
         <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11">
         <v>25</v>
@@ -3143,7 +3162,7 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3152,14 +3171,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3176,7 +3195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3184,7 +3203,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2">
         <v>20</v>
@@ -3193,10 +3212,10 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3204,7 +3223,7 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -3213,10 +3232,10 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3224,7 +3243,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -3233,10 +3252,10 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3244,7 +3263,7 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5">
         <v>30</v>
@@ -3253,10 +3272,10 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3264,7 +3283,7 @@
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6">
         <v>15</v>
@@ -3273,10 +3292,10 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3284,7 +3303,7 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -3293,10 +3312,10 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3304,7 +3323,7 @@
         <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8">
         <v>15</v>
@@ -3313,10 +3332,10 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3324,7 +3343,7 @@
         <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -3333,7 +3352,7 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -3342,14 +3361,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3366,7 +3385,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3374,7 +3393,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -3383,10 +3402,10 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3394,7 +3413,7 @@
         <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -3403,10 +3422,10 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3414,7 +3433,7 @@
         <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4">
         <v>15</v>
@@ -3423,10 +3442,10 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3434,7 +3453,7 @@
         <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D5">
         <v>30</v>
@@ -3443,10 +3462,10 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3454,7 +3473,7 @@
         <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -3463,10 +3482,10 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3474,7 +3493,7 @@
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7">
         <v>20</v>
@@ -3483,10 +3502,10 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3494,7 +3513,7 @@
         <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8">
         <v>20</v>
@@ -3503,10 +3522,10 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3514,7 +3533,7 @@
         <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -3523,10 +3542,10 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3534,7 +3553,7 @@
         <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D10">
         <v>20</v>
@@ -3543,10 +3562,10 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3554,7 +3573,7 @@
         <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11">
         <v>15</v>
@@ -3563,7 +3582,7 @@
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3572,14 +3591,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3596,7 +3615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3604,7 +3623,7 @@
         <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D2">
         <v>15</v>
@@ -3613,10 +3632,10 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3624,7 +3643,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -3633,10 +3652,10 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3644,7 +3663,7 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4">
         <v>20</v>
@@ -3653,10 +3672,10 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3664,7 +3683,7 @@
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5">
         <v>25</v>
@@ -3673,10 +3692,10 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3684,7 +3703,7 @@
         <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6">
         <v>30</v>
@@ -3693,10 +3712,10 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3704,7 +3723,7 @@
         <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7">
         <v>15</v>
@@ -3713,10 +3732,10 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3724,7 +3743,7 @@
         <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -3733,10 +3752,10 @@
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3744,7 +3763,7 @@
         <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -3753,10 +3772,10 @@
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3764,7 +3783,7 @@
         <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10">
         <v>15</v>
@@ -3773,7 +3792,7 @@
         <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3782,14 +3801,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3806,7 +3825,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3814,7 +3833,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2">
         <v>15</v>
@@ -3823,10 +3842,10 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3834,7 +3853,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3">
         <v>15</v>
@@ -3843,10 +3862,10 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3854,7 +3873,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -3863,10 +3882,10 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3874,7 +3893,7 @@
         <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5">
         <v>30</v>
@@ -3883,10 +3902,10 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3894,7 +3913,7 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6">
         <v>10</v>
@@ -3903,10 +3922,10 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3914,7 +3933,7 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7">
         <v>20</v>
@@ -3923,10 +3942,10 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3934,7 +3953,7 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -3943,10 +3962,10 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3954,7 +3973,7 @@
         <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9">
         <v>15</v>
@@ -3963,10 +3982,10 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3974,7 +3993,7 @@
         <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10">
         <v>20</v>
@@ -3983,7 +4002,7 @@
         <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalized program fully completed
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -385,31 +385,31 @@
     <t>For March, the school limit for IAIM is reached</t>
   </si>
   <si>
-    <t>For  February, the 10-minute slot is unavailable</t>
-  </si>
-  <si>
-    <t>For  June, the 10-minute slot is unavailable</t>
-  </si>
-  <si>
-    <t>For  February, the 15-minute slot is unavailable</t>
-  </si>
-  <si>
-    <t>For  April, the 30-minute slot is unavailable</t>
-  </si>
-  <si>
-    <t>For  March, the 30-minute slot is unavailable</t>
-  </si>
-  <si>
-    <t>For  June, the 30-minute slot is unavailable</t>
-  </si>
-  <si>
-    <t>For  May, the 30-minute slot is unavailable</t>
-  </si>
-  <si>
-    <t>For  March, the 10-minute slot is unavailable</t>
-  </si>
-  <si>
-    <t>For  April, the 10-minute slot is unavailable</t>
+    <t>For February, the 10-minute slot is unavailable</t>
+  </si>
+  <si>
+    <t>For June, the 10-minute slot is unavailable</t>
+  </si>
+  <si>
+    <t>For February, the 15-minute slot is unavailable</t>
+  </si>
+  <si>
+    <t>For April, the 30-minute slot is unavailable</t>
+  </si>
+  <si>
+    <t>For March, the 30-minute slot is unavailable</t>
+  </si>
+  <si>
+    <t>For June, the 30-minute slot is unavailable</t>
+  </si>
+  <si>
+    <t>For May, the 30-minute slot is unavailable</t>
+  </si>
+  <si>
+    <t>For March, the 10-minute slot is unavailable</t>
+  </si>
+  <si>
+    <t>For April, the 10-minute slot is unavailable</t>
   </si>
   <si>
     <t>The performer's ability to perform in this half is uncertain</t>

</xml_diff>